<commit_message>
added support for named variables
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -355,7 +355,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -391,6 +391,10 @@
       <c r="C2">
         <f t="shared" si="1"/>
         <v>-0.99177885344311578</v>
+      </c>
+      <c r="D2">
+        <f>D1+SINUS</f>
+        <v>-1.0146426216161242</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>

<commit_message>
update functions set and call
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,13 +67,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -355,7 +383,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -443,6 +471,10 @@
         <f t="shared" si="1"/>
         <v>-0.68328372503552359</v>
       </c>
+      <c r="D5">
+        <f>MATCH(3,A1:A18,0)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
@@ -615,6 +647,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
add offset function and : operator but cellmap needs to include all cells (tbc)
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,8 +67,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -79,13 +87,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,61 +396,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <f t="shared" ref="B1:B18" si="0">SUM(A1:A3)</f>
-        <v>6</v>
+        <f>SUM(A1:A3)+B2</f>
+        <v>15</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:C18" si="1">SIN(B1*A1^2)</f>
-        <v>-0.27941549819892586</v>
+        <f t="shared" ref="C1:C18" si="0">SIN(B1*A1^2)</f>
+        <v>0.65028784015711683</v>
       </c>
       <c r="D1">
         <f>LINEST(C1:C18,B1:B18)</f>
-        <v>-2.2863768173008364E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>-3.0552273458940418E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B1:B18" si="1">SUM(A2:A4)</f>
         <v>9</v>
       </c>
       <c r="C2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.99177885344311578</v>
       </c>
       <c r="D2">
         <f>D1+SINUS</f>
-        <v>-1.0146426216161242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>-1.0223311269020563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="C3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.92681850541778499</v>
       </c>
       <c r="D3">
@@ -442,16 +456,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.9454451549211168</v>
       </c>
       <c r="D4">
@@ -459,16 +473,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.68328372503552359</v>
       </c>
       <c r="D5">
@@ -476,146 +490,158 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.90176229056057366</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.86459689169594789</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.12372268789623808</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.99975982007864272</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9">
+        <f ca="1">SUM(A1:OFFSET(A2,A4,0))</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.97060061981194778</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10">
+        <f ca="1">SUM(A2:OFFSET(A3,4,0))</f>
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <f ca="1">INDIRECT(ADDRESS(2,2))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.98352241357378278</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>12</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.91983693466953753</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>13</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.90954815110388421</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>14</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.9997715643824282</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>15</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.71424378349544093</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>16</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.44311307948133072</v>
       </c>
     </row>
@@ -624,11 +650,11 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.80062916411734009</v>
       </c>
     </row>
@@ -637,11 +663,11 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.93349358571214391</v>
       </c>
     </row>
@@ -658,12 +684,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <f ca="1">SUM(A:A 1:1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <f>SUM(B5:B15 A7:D7)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
allow empty cells when evaluate
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -398,7 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -411,15 +413,15 @@
       </c>
       <c r="B1">
         <f>SUM(A1:A3)+B2</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C1">
-        <f t="shared" ref="C1:C18" si="0">SIN(B1*A1^2)</f>
-        <v>0.65028784015711683</v>
+        <f t="shared" ref="C1:C21" si="0">SIN(B1*A1^2)</f>
+        <v>-0.40403764532306502</v>
       </c>
       <c r="D1">
         <f>LINEST(C1:C18,B1:B18)</f>
-        <v>-3.0552273458940418E-2</v>
+        <v>-3.8320733871814408E-2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -427,16 +429,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B1:B18" si="1">SUM(A2:A4)</f>
-        <v>9</v>
+        <f t="shared" ref="B1:B21" si="1">SUM(A2:A4)</f>
+        <v>25</v>
       </c>
       <c r="C2">
         <f t="shared" si="0"/>
-        <v>-0.99177885344311578</v>
+        <v>-0.50636564110975879</v>
       </c>
       <c r="D2">
         <f>D1+SINUS</f>
-        <v>-1.0223311269020563</v>
+        <v>-0.54468637498157324</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -445,28 +447,28 @@
       </c>
       <c r="B3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>0.92681850541778499</v>
+        <v>0.623012211003653</v>
       </c>
       <c r="D3">
         <f ca="1">OFFSET(A1,1,1)</f>
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.9454451549211168</v>
+        <v>-0.13339744711461884</v>
       </c>
       <c r="D4">
         <f>MATCH(3,A1:A18,0)</f>
@@ -542,8 +544,8 @@
         <v>-0.99975982007864272</v>
       </c>
       <c r="D9">
-        <f ca="1">SUM(A1:OFFSET(A2,A4,0))</f>
-        <v>21</v>
+        <f ca="1">SUM(A1:OFFSET(A2,A4*2,0))</f>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -560,11 +562,11 @@
       </c>
       <c r="D10">
         <f ca="1">SUM(A2:OFFSET(A3,4,0))</f>
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E10">
         <f ca="1">INDIRECT(ADDRESS(2,2))</f>
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5">

</xml_diff>